<commit_message>
value-driven dataset & analysis corr.
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-7.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-7.xlsx
@@ -72,7 +72,7 @@
     <t>Кол-во нулей</t>
   </si>
   <si>
-    <t>Анализ признаков в датасете (размер выборки +1900 примеров)</t>
+    <t>Анализ признаков в датасете (размер выборки 1925 примеров)</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1310,7 @@
   <dimension ref="C3:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="P5" s="4">
-        <v>586.64</v>
+        <v>601.5</v>
       </c>
       <c r="Q5" s="4">
         <v>38482</v>
@@ -1384,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="4">
-        <v>937</v>
+        <v>888</v>
       </c>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>8</v>
       </c>
       <c r="P6" s="4">
-        <v>34.07</v>
+        <v>38.01</v>
       </c>
       <c r="Q6" s="4">
         <v>359</v>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="4">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>9</v>
       </c>
       <c r="P7" s="4">
-        <v>44.48</v>
+        <v>45.61</v>
       </c>
       <c r="Q7" s="4">
         <v>730</v>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="4">
-        <v>811</v>
+        <v>762</v>
       </c>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
         <v>10</v>
       </c>
       <c r="P8" s="4">
-        <v>0.57999999999999996</v>
+        <v>0.59</v>
       </c>
       <c r="Q8" s="4">
         <v>35</v>
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="4">
-        <v>1278</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="P9" s="4">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="Q9" s="4">
         <v>4</v>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="4">
-        <v>1646</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="4">
-        <v>1746</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">

</xml_diff>